<commit_message>
2022/12/2 version_edit exist problem(beds, sbrecords, rollcalls, lates)
</commit_message>
<xml_diff>
--- a/第一組宿舍管理系統.xlsx
+++ b/第一組宿舍管理系統.xlsx
@@ -1,35 +1,49 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\team01\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB29E8B-AFAD-4D50-A8CA-D2673A6C07BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7950" firstSheet="10" activeTab="15"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="10" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="學生資料表" sheetId="1" r:id="rId1"/>
     <sheet name="床位資料表" sheetId="3" r:id="rId2"/>
     <sheet name="宿舍資料表" sheetId="5" r:id="rId3"/>
     <sheet name="學生床位資料表" sheetId="7" r:id="rId4"/>
-    <sheet name="外宿申請表" sheetId="9" r:id="rId5"/>
+    <sheet name="點名資料表" sheetId="13" r:id="rId5"/>
     <sheet name="長期晚歸申請表" sheetId="11" r:id="rId6"/>
-    <sheet name="點名資料表" sheetId="13" r:id="rId7"/>
+    <sheet name="外宿申請表" sheetId="9" r:id="rId7"/>
     <sheet name="人臉資料表" sheetId="15" r:id="rId8"/>
     <sheet name="學生表格(students)" sheetId="2" r:id="rId9"/>
-    <sheet name="宿舍表格(dormitories)" sheetId="6" r:id="rId10"/>
-    <sheet name="床位表格(beds)" sheetId="4" r:id="rId11"/>
+    <sheet name="床位表格(beds)" sheetId="4" r:id="rId10"/>
+    <sheet name="宿舍表格(dormitories)" sheetId="6" r:id="rId11"/>
     <sheet name="學生床位資料表(sbrecords)" sheetId="8" r:id="rId12"/>
     <sheet name="點名表格(rollcalls)" sheetId="14" r:id="rId13"/>
-    <sheet name="外宿表格(leaves)" sheetId="10" r:id="rId14"/>
-    <sheet name="長期晚歸表格(lates)" sheetId="12" r:id="rId15"/>
+    <sheet name="長期晚歸表格(lates)" sheetId="12" r:id="rId14"/>
+    <sheet name="外宿表格(leaves)" sheetId="10" r:id="rId15"/>
     <sheet name="人臉表格(features)" sheetId="16" r:id="rId16"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1266,11 +1280,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="176" formatCode="m/d"/>
-    <numFmt numFmtId="186" formatCode="0_);\(0\)"/>
-    <numFmt numFmtId="192" formatCode="#,##0.0000000"/>
+    <numFmt numFmtId="177" formatCode="0_);\(0\)"/>
+    <numFmt numFmtId="178" formatCode="#,##0.0000000"/>
   </numFmts>
   <fonts count="17">
     <font>
@@ -1795,20 +1809,20 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="186" fontId="5" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="5" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="186" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="186" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="186" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="192" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -2112,7 +2126,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -3178,34 +3192,8 @@
       <c r="K32"/>
       <c r="L32"/>
     </row>
-    <row r="33" spans="1:12">
-      <c r="A33"/>
-      <c r="B33"/>
-      <c r="C33"/>
-      <c r="D33"/>
-      <c r="E33"/>
-      <c r="F33"/>
-      <c r="G33"/>
-      <c r="H33"/>
-      <c r="I33"/>
-      <c r="J33"/>
-      <c r="K33"/>
-      <c r="L33"/>
-    </row>
-    <row r="34" spans="1:12">
-      <c r="A34"/>
-      <c r="B34"/>
-      <c r="C34"/>
-      <c r="D34"/>
-      <c r="E34"/>
-      <c r="F34"/>
-      <c r="G34"/>
-      <c r="H34"/>
-      <c r="I34"/>
-      <c r="J34"/>
-      <c r="K34"/>
-      <c r="L34"/>
-    </row>
+    <row r="33" customFormat="1"/>
+    <row r="34" customFormat="1"/>
   </sheetData>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3213,7 +3201,172 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" style="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A3" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A4" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="8"/>
+    </row>
+    <row r="5" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A5" s="68" t="s">
+        <v>306</v>
+      </c>
+      <c r="B5" s="68" t="s">
+        <v>307</v>
+      </c>
+      <c r="C5" s="68" t="s">
+        <v>308</v>
+      </c>
+      <c r="D5" s="68"/>
+      <c r="E5" s="69" t="s">
+        <v>309</v>
+      </c>
+      <c r="F5" s="70"/>
+    </row>
+    <row r="6" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A6" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A7" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="8"/>
+    </row>
+    <row r="8" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="8"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="10" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -3359,179 +3512,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:F8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
-  <cols>
-    <col min="1" max="1" width="16.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" style="10" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A3" s="35" t="s">
-        <v>96</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="7"/>
-    </row>
-    <row r="4" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A4" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="8"/>
-    </row>
-    <row r="5" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A5" s="68" t="s">
-        <v>306</v>
-      </c>
-      <c r="B5" s="68" t="s">
-        <v>307</v>
-      </c>
-      <c r="C5" s="68" t="s">
-        <v>308</v>
-      </c>
-      <c r="D5" s="68"/>
-      <c r="E5" s="69" t="s">
-        <v>309</v>
-      </c>
-      <c r="F5" s="70"/>
-    </row>
-    <row r="6" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A6" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="7"/>
-    </row>
-    <row r="7" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A7" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="8"/>
-    </row>
-    <row r="8" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A8" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="8"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -3726,7 +3714,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -3914,7 +3902,319 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="22.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.140625" style="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A8" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A9" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A10" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A11" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A12" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A13" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A14" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A15" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="7"/>
+    </row>
+    <row r="16" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A16" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="8"/>
+    </row>
+    <row r="17" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A17" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="8"/>
+      <c r="E17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="8"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="10" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -4110,326 +4410,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:F17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
-  <cols>
-    <col min="1" max="1" width="22.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.140625" style="10" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="7"/>
-    </row>
-    <row r="5" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A5" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A6" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="7"/>
-    </row>
-    <row r="7" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A7" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A8" s="5" t="s">
-        <v>316</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="7"/>
-    </row>
-    <row r="9" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A9" s="5" t="s">
-        <v>324</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="7"/>
-    </row>
-    <row r="10" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A10" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="7"/>
-    </row>
-    <row r="11" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A11" s="5" t="s">
-        <v>323</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="7"/>
-    </row>
-    <row r="12" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A12" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>321</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="7"/>
-    </row>
-    <row r="13" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A13" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>322</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="7"/>
-    </row>
-    <row r="14" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A14" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>311</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="7"/>
-    </row>
-    <row r="15" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A15" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="7"/>
-    </row>
-    <row r="16" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A16" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="8"/>
-    </row>
-    <row r="17" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A17" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F17" s="8"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -4573,14 +4561,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:G134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G34" sqref="A32:G34"/>
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -5630,7 +5618,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -5744,7 +5732,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -5796,7 +5784,7 @@
     </row>
     <row r="2" spans="1:9" ht="18.75" customHeight="1">
       <c r="A2" s="16">
-        <f t="shared" ref="A2:A37" si="0">ROW()-1</f>
+        <f t="shared" ref="A2:A31" si="0">ROW()-1</f>
         <v>1</v>
       </c>
       <c r="B2" s="16">
@@ -6441,7 +6429,879 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:I34"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" style="56" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="6" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.5703125" style="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="18.75" customHeight="1">
+      <c r="A1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="58" t="s">
+        <v>299</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="18.75" customHeight="1">
+      <c r="A2" s="16">
+        <f t="shared" ref="A2:A31" si="0">ROW()-1</f>
+        <v>1</v>
+      </c>
+      <c r="B2" s="17">
+        <v>44847</v>
+      </c>
+      <c r="C2" s="55">
+        <v>1</v>
+      </c>
+      <c r="D2" s="16">
+        <v>1</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+    </row>
+    <row r="3" spans="1:9" ht="18.75" customHeight="1">
+      <c r="A3" s="16">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B3" s="17">
+        <v>44847</v>
+      </c>
+      <c r="C3" s="55">
+        <v>1</v>
+      </c>
+      <c r="D3" s="16">
+        <v>2</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+    </row>
+    <row r="4" spans="1:9" ht="18.75" customHeight="1">
+      <c r="A4" s="16">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B4" s="17">
+        <v>44847</v>
+      </c>
+      <c r="C4" s="55">
+        <v>1</v>
+      </c>
+      <c r="D4" s="16">
+        <v>3</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+    </row>
+    <row r="5" spans="1:9" ht="18.75" customHeight="1">
+      <c r="A5" s="16">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="17">
+        <v>44847</v>
+      </c>
+      <c r="C5" s="55">
+        <v>1</v>
+      </c>
+      <c r="D5" s="16">
+        <v>4</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+    </row>
+    <row r="6" spans="1:9" ht="18.75" customHeight="1">
+      <c r="A6" s="16">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="17">
+        <v>44847</v>
+      </c>
+      <c r="C6" s="55">
+        <v>1</v>
+      </c>
+      <c r="D6" s="16">
+        <v>5</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+    </row>
+    <row r="7" spans="1:9" ht="18.75" customHeight="1">
+      <c r="A7" s="16">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="17">
+        <v>44847</v>
+      </c>
+      <c r="C7" s="55">
+        <v>1</v>
+      </c>
+      <c r="D7" s="16">
+        <v>6</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+    </row>
+    <row r="8" spans="1:9" ht="18.75" customHeight="1">
+      <c r="A8" s="16">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="17">
+        <v>44847</v>
+      </c>
+      <c r="C8" s="55">
+        <v>1</v>
+      </c>
+      <c r="D8" s="16">
+        <v>7</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+    </row>
+    <row r="9" spans="1:9" ht="18.75" customHeight="1">
+      <c r="A9" s="16">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="17">
+        <v>44847</v>
+      </c>
+      <c r="C9" s="55">
+        <v>1</v>
+      </c>
+      <c r="D9" s="16">
+        <v>8</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+    </row>
+    <row r="10" spans="1:9" ht="18.75" customHeight="1">
+      <c r="A10" s="16">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="17">
+        <v>44847</v>
+      </c>
+      <c r="C10" s="55">
+        <v>1</v>
+      </c>
+      <c r="D10" s="16">
+        <v>9</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+    </row>
+    <row r="11" spans="1:9" ht="18.75" customHeight="1">
+      <c r="A11" s="16">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="17">
+        <v>44847</v>
+      </c>
+      <c r="C11" s="55">
+        <v>1</v>
+      </c>
+      <c r="D11" s="16">
+        <v>10</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="16">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="17">
+        <v>44847</v>
+      </c>
+      <c r="C12" s="55">
+        <v>1</v>
+      </c>
+      <c r="D12" s="16">
+        <v>11</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="16">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="17">
+        <v>44847</v>
+      </c>
+      <c r="C13" s="55">
+        <v>1</v>
+      </c>
+      <c r="D13" s="16">
+        <v>12</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="16">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="17">
+        <v>44847</v>
+      </c>
+      <c r="C14" s="57">
+        <v>1</v>
+      </c>
+      <c r="D14" s="16">
+        <v>13</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="16">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="17">
+        <v>44847</v>
+      </c>
+      <c r="C15" s="57">
+        <v>1</v>
+      </c>
+      <c r="D15" s="16">
+        <v>14</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="17">
+        <v>44847</v>
+      </c>
+      <c r="C16" s="57">
+        <v>1</v>
+      </c>
+      <c r="D16" s="16">
+        <v>15</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="16">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="17">
+        <v>44847</v>
+      </c>
+      <c r="C17" s="57">
+        <v>1</v>
+      </c>
+      <c r="D17" s="16">
+        <v>16</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="16">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="17">
+        <v>44847</v>
+      </c>
+      <c r="C18" s="57">
+        <v>1</v>
+      </c>
+      <c r="D18" s="16">
+        <v>17</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="16">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="17">
+        <v>44847</v>
+      </c>
+      <c r="C19" s="57">
+        <v>1</v>
+      </c>
+      <c r="D19" s="16">
+        <v>18</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="16">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="17">
+        <v>44847</v>
+      </c>
+      <c r="C20" s="57">
+        <v>1</v>
+      </c>
+      <c r="D20" s="16">
+        <v>19</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="16">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="17">
+        <v>44847</v>
+      </c>
+      <c r="C21" s="57">
+        <v>1</v>
+      </c>
+      <c r="D21" s="16">
+        <v>20</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="16">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="17">
+        <v>44847</v>
+      </c>
+      <c r="C22" s="57">
+        <v>1</v>
+      </c>
+      <c r="D22" s="16">
+        <v>21</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="16">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B23" s="17">
+        <v>44847</v>
+      </c>
+      <c r="C23" s="57">
+        <v>1</v>
+      </c>
+      <c r="D23" s="16">
+        <v>22</v>
+      </c>
+      <c r="E23" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="16">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="17">
+        <v>44847</v>
+      </c>
+      <c r="C24" s="57">
+        <v>1</v>
+      </c>
+      <c r="D24" s="16">
+        <v>23</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="16">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B25" s="17">
+        <v>44847</v>
+      </c>
+      <c r="C25" s="57">
+        <v>1</v>
+      </c>
+      <c r="D25" s="16">
+        <v>24</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="16">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="17">
+        <v>44847</v>
+      </c>
+      <c r="C26" s="57">
+        <v>1</v>
+      </c>
+      <c r="D26" s="16">
+        <v>25</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="16">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B27" s="17">
+        <v>44847</v>
+      </c>
+      <c r="C27" s="57">
+        <v>1</v>
+      </c>
+      <c r="D27" s="16">
+        <v>26</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="16">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B28" s="17">
+        <v>44847</v>
+      </c>
+      <c r="C28" s="57">
+        <v>1</v>
+      </c>
+      <c r="D28" s="16">
+        <v>27</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="16">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B29" s="17">
+        <v>44847</v>
+      </c>
+      <c r="C29" s="57">
+        <v>1</v>
+      </c>
+      <c r="D29" s="16">
+        <v>28</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="16">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B30" s="17">
+        <v>44847</v>
+      </c>
+      <c r="C30" s="57">
+        <v>1</v>
+      </c>
+      <c r="D30" s="16">
+        <v>29</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="16">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B31" s="17">
+        <v>44847</v>
+      </c>
+      <c r="C31" s="57">
+        <v>1</v>
+      </c>
+      <c r="D31" s="16">
+        <v>30</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="18"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32"/>
+      <c r="F32"/>
+      <c r="G32"/>
+      <c r="H32"/>
+      <c r="I32"/>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="18"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33"/>
+      <c r="F33"/>
+      <c r="G33"/>
+      <c r="H33"/>
+      <c r="I33"/>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="18"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34"/>
+      <c r="F34"/>
+      <c r="G34"/>
+      <c r="H34"/>
+      <c r="I34"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="10" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:Q3"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="15" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.42578125" style="26" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="15" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="11" style="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="18.75" customHeight="1">
+      <c r="A1" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>325</v>
+      </c>
+      <c r="G1" s="72" t="s">
+        <v>315</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>324</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="N1" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="O1" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="P1" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="18.75" customHeight="1">
+      <c r="A2" s="16">
+        <f>ROW()-1</f>
+        <v>1</v>
+      </c>
+      <c r="B2" s="16">
+        <v>6</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="I2" s="25">
+        <v>1.9791666666666665</v>
+      </c>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+    </row>
+    <row r="3" spans="1:17" ht="18.75" customHeight="1">
+      <c r="A3" s="16">
+        <f>ROW()-1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="16">
+        <v>7</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="I3" s="25">
+        <v>0</v>
+      </c>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="19"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="10" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -6541,880 +7401,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:Q3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
-  <cols>
-    <col min="1" max="1" width="12.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="15" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.42578125" style="26" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="15" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11" style="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="11" style="10" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17" ht="18.75" customHeight="1">
-      <c r="A1" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="23" t="s">
-        <v>325</v>
-      </c>
-      <c r="G1" s="72" t="s">
-        <v>315</v>
-      </c>
-      <c r="H1" s="23" t="s">
-        <v>324</v>
-      </c>
-      <c r="I1" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="K1" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="L1" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="M1" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="N1" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="O1" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="P1" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q1" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="18.75" customHeight="1">
-      <c r="A2" s="16">
-        <f>ROW()-1</f>
-        <v>1</v>
-      </c>
-      <c r="B2" s="16">
-        <v>6</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="I2" s="25">
-        <v>1.9791666666666665</v>
-      </c>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-    </row>
-    <row r="3" spans="1:17" ht="18.75" customHeight="1">
-      <c r="A3" s="16">
-        <f>ROW()-1</f>
-        <v>2</v>
-      </c>
-      <c r="B3" s="16">
-        <v>7</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="H3" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="I3" s="25">
-        <v>0</v>
-      </c>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19"/>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="19"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:I34"/>
-  <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E34" sqref="A32:E34"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
-  <cols>
-    <col min="1" max="1" width="13.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" style="56" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="6" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="13.5703125" style="10" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A1" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="58" t="s">
-        <v>299</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="I1" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A2" s="16">
-        <f t="shared" ref="A2:A31" si="0">ROW()-1</f>
-        <v>1</v>
-      </c>
-      <c r="B2" s="17">
-        <v>44847</v>
-      </c>
-      <c r="C2" s="55">
-        <v>1</v>
-      </c>
-      <c r="D2" s="16">
-        <v>1</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-    </row>
-    <row r="3" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A3" s="16">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="B3" s="17">
-        <v>44847</v>
-      </c>
-      <c r="C3" s="55">
-        <v>1</v>
-      </c>
-      <c r="D3" s="16">
-        <v>2</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-    </row>
-    <row r="4" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A4" s="16">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="B4" s="17">
-        <v>44847</v>
-      </c>
-      <c r="C4" s="55">
-        <v>1</v>
-      </c>
-      <c r="D4" s="16">
-        <v>3</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-    </row>
-    <row r="5" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A5" s="16">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B5" s="17">
-        <v>44847</v>
-      </c>
-      <c r="C5" s="55">
-        <v>1</v>
-      </c>
-      <c r="D5" s="16">
-        <v>4</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-    </row>
-    <row r="6" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A6" s="16">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B6" s="17">
-        <v>44847</v>
-      </c>
-      <c r="C6" s="55">
-        <v>1</v>
-      </c>
-      <c r="D6" s="16">
-        <v>5</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-    </row>
-    <row r="7" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A7" s="16">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B7" s="17">
-        <v>44847</v>
-      </c>
-      <c r="C7" s="55">
-        <v>1</v>
-      </c>
-      <c r="D7" s="16">
-        <v>6</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-    </row>
-    <row r="8" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A8" s="16">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B8" s="17">
-        <v>44847</v>
-      </c>
-      <c r="C8" s="55">
-        <v>1</v>
-      </c>
-      <c r="D8" s="16">
-        <v>7</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-    </row>
-    <row r="9" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A9" s="16">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B9" s="17">
-        <v>44847</v>
-      </c>
-      <c r="C9" s="55">
-        <v>1</v>
-      </c>
-      <c r="D9" s="16">
-        <v>8</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-    </row>
-    <row r="10" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A10" s="16">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B10" s="17">
-        <v>44847</v>
-      </c>
-      <c r="C10" s="55">
-        <v>1</v>
-      </c>
-      <c r="D10" s="16">
-        <v>9</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-    </row>
-    <row r="11" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A11" s="16">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B11" s="17">
-        <v>44847</v>
-      </c>
-      <c r="C11" s="55">
-        <v>1</v>
-      </c>
-      <c r="D11" s="16">
-        <v>10</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="16">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B12" s="17">
-        <v>44847</v>
-      </c>
-      <c r="C12" s="55">
-        <v>1</v>
-      </c>
-      <c r="D12" s="16">
-        <v>11</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="16">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="B13" s="17">
-        <v>44847</v>
-      </c>
-      <c r="C13" s="55">
-        <v>1</v>
-      </c>
-      <c r="D13" s="16">
-        <v>12</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="16">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="B14" s="17">
-        <v>44847</v>
-      </c>
-      <c r="C14" s="57">
-        <v>1</v>
-      </c>
-      <c r="D14" s="16">
-        <v>13</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="16">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="B15" s="17">
-        <v>44847</v>
-      </c>
-      <c r="C15" s="57">
-        <v>1</v>
-      </c>
-      <c r="D15" s="16">
-        <v>14</v>
-      </c>
-      <c r="E15" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="16">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="B16" s="17">
-        <v>44847</v>
-      </c>
-      <c r="C16" s="57">
-        <v>1</v>
-      </c>
-      <c r="D16" s="16">
-        <v>15</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="16">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B17" s="17">
-        <v>44847</v>
-      </c>
-      <c r="C17" s="57">
-        <v>1</v>
-      </c>
-      <c r="D17" s="16">
-        <v>16</v>
-      </c>
-      <c r="E17" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="16">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="B18" s="17">
-        <v>44847</v>
-      </c>
-      <c r="C18" s="57">
-        <v>1</v>
-      </c>
-      <c r="D18" s="16">
-        <v>17</v>
-      </c>
-      <c r="E18" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="16">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="B19" s="17">
-        <v>44847</v>
-      </c>
-      <c r="C19" s="57">
-        <v>1</v>
-      </c>
-      <c r="D19" s="16">
-        <v>18</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="16">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="B20" s="17">
-        <v>44847</v>
-      </c>
-      <c r="C20" s="57">
-        <v>1</v>
-      </c>
-      <c r="D20" s="16">
-        <v>19</v>
-      </c>
-      <c r="E20" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="16">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="B21" s="17">
-        <v>44847</v>
-      </c>
-      <c r="C21" s="57">
-        <v>1</v>
-      </c>
-      <c r="D21" s="16">
-        <v>20</v>
-      </c>
-      <c r="E21" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="16">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="B22" s="17">
-        <v>44847</v>
-      </c>
-      <c r="C22" s="57">
-        <v>1</v>
-      </c>
-      <c r="D22" s="16">
-        <v>21</v>
-      </c>
-      <c r="E22" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="16">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="B23" s="17">
-        <v>44847</v>
-      </c>
-      <c r="C23" s="57">
-        <v>1</v>
-      </c>
-      <c r="D23" s="16">
-        <v>22</v>
-      </c>
-      <c r="E23" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="16">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="B24" s="17">
-        <v>44847</v>
-      </c>
-      <c r="C24" s="57">
-        <v>1</v>
-      </c>
-      <c r="D24" s="16">
-        <v>23</v>
-      </c>
-      <c r="E24" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="16">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="B25" s="17">
-        <v>44847</v>
-      </c>
-      <c r="C25" s="57">
-        <v>1</v>
-      </c>
-      <c r="D25" s="16">
-        <v>24</v>
-      </c>
-      <c r="E25" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="16">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="B26" s="17">
-        <v>44847</v>
-      </c>
-      <c r="C26" s="57">
-        <v>1</v>
-      </c>
-      <c r="D26" s="16">
-        <v>25</v>
-      </c>
-      <c r="E26" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="16">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="B27" s="17">
-        <v>44847</v>
-      </c>
-      <c r="C27" s="57">
-        <v>1</v>
-      </c>
-      <c r="D27" s="16">
-        <v>26</v>
-      </c>
-      <c r="E27" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="16">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="B28" s="17">
-        <v>44847</v>
-      </c>
-      <c r="C28" s="57">
-        <v>1</v>
-      </c>
-      <c r="D28" s="16">
-        <v>27</v>
-      </c>
-      <c r="E28" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="16">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="B29" s="17">
-        <v>44847</v>
-      </c>
-      <c r="C29" s="57">
-        <v>1</v>
-      </c>
-      <c r="D29" s="16">
-        <v>28</v>
-      </c>
-      <c r="E29" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="16">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="B30" s="17">
-        <v>44847</v>
-      </c>
-      <c r="C30" s="57">
-        <v>1</v>
-      </c>
-      <c r="D30" s="16">
-        <v>29</v>
-      </c>
-      <c r="E30" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="16">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="B31" s="17">
-        <v>44847</v>
-      </c>
-      <c r="C31" s="57">
-        <v>1</v>
-      </c>
-      <c r="D31" s="16">
-        <v>30</v>
-      </c>
-      <c r="E31" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="18"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32"/>
-      <c r="F32"/>
-      <c r="G32"/>
-      <c r="H32"/>
-      <c r="I32"/>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33" s="18"/>
-      <c r="B33" s="18"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33"/>
-      <c r="F33"/>
-      <c r="G33"/>
-      <c r="H33"/>
-      <c r="I33"/>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34" s="18"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34"/>
-      <c r="F34"/>
-      <c r="G34"/>
-      <c r="H34"/>
-      <c r="I34"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="工作表1">
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -8026,7 +8014,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>

</xml_diff>